<commit_message>
Update data package at: 2024-09-26T19:02:18Z
</commit_message>
<xml_diff>
--- a/data-raw/desc_IPU.xlsx
+++ b/data-raw/desc_IPU.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26914"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m1529042\Desktop\2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="11_B288C9EF925CD735DDB2D4C730626BB5276C6FF8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="11_B288C9EF925CD735DDB2D4C730626BB5276C6FF8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B217E22E-31ED-4597-80A4-3EAA4C17F5A9}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="8400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,11 +19,22 @@
     <definedName name="_Toc421621627" localSheetId="0">'Idenficadores de procedência e '!#REF!</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
@@ -58,7 +69,7 @@
     <t>RECURSOS RECEBIDOS PARA CONTRAPARTIDA DE OPERAÇÃO DE CRÉDITO</t>
   </si>
   <si>
-    <t>RECURSOS RECEBIDOS PARA AUXÍLIOS DOENÇA, FUNERAL, ALIMENTAÇÃO, TRANSPORTE E FARDAMENTO</t>
+    <t>RECURSOS RECEBIDOS PARA AUXÍLIOS</t>
   </si>
   <si>
     <t>RECURSOS RECEBIDOS PARA EMENDAS PARLAMENTARES</t>
@@ -385,7 +396,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -743,6 +754,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="b91e7f20-fe0a-487d-91a9-605ac1c64acf" xsi:nil="true"/>
@@ -760,23 +780,14 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{83CCCF36-5B33-4B61-A5C7-201737F69C59}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0A2C736-546E-484E-93B3-B1A0CB59FCDC}"/>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38DFFBB6-78D5-4692-BD04-46A377810F60}"/>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0A2C736-546E-484E-93B3-B1A0CB59FCDC}"/>
 </file>
</xml_diff>